<commit_message>
Random Forest grid param testing #5
Random Forest grid param testing #6 - IN PROGRESS
</commit_message>
<xml_diff>
--- a/code/random_forest-outfiles/RFECV 1 2 3 4.xlsx
+++ b/code/random_forest-outfiles/RFECV 1 2 3 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Research-Spring2021\code\random_forest-outfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FB7E3E-1CCD-489A-A1D4-02EA8D662C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161D59B8-3027-468D-AA16-7DC364ED3E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2478,7 +2477,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>